<commit_message>
upload siswa + create read delete anggota
</commit_message>
<xml_diff>
--- a/requirement/action plan.xlsx
+++ b/requirement/action plan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\KULIAH\SEMESTER 6\1A_Project\perpus wb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VFAIROH\Documents\semester 6\perpus-wb\requirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF3BE26-1380-4524-B5FF-7D192170303D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -242,7 +237,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -363,11 +358,13 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -375,20 +372,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,11 +697,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,35 +714,35 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -772,10 +767,10 @@
         <v>43899</v>
       </c>
       <c r="H5" s="5"/>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="12" t="s">
         <v>22</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -801,8 +796,8 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="19" t="s">
+      <c r="J6" s="19"/>
+      <c r="K6" s="12" t="s">
         <v>23</v>
       </c>
       <c r="L6" s="1" t="s">
@@ -810,18 +805,18 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="19" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="12" t="s">
         <v>24</v>
       </c>
       <c r="L7" s="1" t="s">
@@ -851,8 +846,8 @@
         <v>43901</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="19" t="s">
+      <c r="J8" s="19"/>
+      <c r="K8" s="12" t="s">
         <v>25</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -1004,7 +999,9 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <v>10</v>
+      </c>
       <c r="B15" s="1" t="s">
         <v>58</v>
       </c>
@@ -1026,7 +1023,9 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1">
+        <v>11</v>
+      </c>
       <c r="B16" s="1" t="s">
         <v>59</v>
       </c>
@@ -1049,7 +1048,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>36</v>
@@ -1072,20 +1071,20 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>43</v>
@@ -1109,7 +1108,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>41</v>
@@ -1133,7 +1132,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>42</v>
@@ -1157,7 +1156,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>48</v>
@@ -1181,7 +1180,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>44</v>
@@ -1205,7 +1204,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>45</v>
@@ -1229,7 +1228,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>46</v>
@@ -1253,7 +1252,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>49</v>
@@ -1277,7 +1276,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>50</v>
@@ -1301,7 +1300,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>54</v>
@@ -1322,20 +1321,20 @@
       <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>55</v>
@@ -1359,7 +1358,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>57</v>
@@ -1383,7 +1382,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>56</v>
@@ -1407,7 +1406,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>60</v>
@@ -1431,7 +1430,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>61</v>
@@ -1455,7 +1454,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>62</v>
@@ -1479,7 +1478,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>63</v>
@@ -1503,7 +1502,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>64</v>
@@ -1526,34 +1525,34 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="14">
-        <v>29</v>
-      </c>
-      <c r="B39" s="14" t="s">
+      <c r="A39" s="11">
+        <v>31</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
+      <c r="D39" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>